<commit_message>
fix bug add and upload users
</commit_message>
<xml_diff>
--- a/downloads/template users.xlsx
+++ b/downloads/template users.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\elearning\downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>First Name</t>
   </si>
@@ -42,6 +37,9 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Username</t>
   </si>
 </sst>
 </file>
@@ -139,7 +137,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -174,7 +172,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -351,7 +349,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -359,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -370,7 +368,7 @@
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,20 +379,23 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" error="Minimal 8 karakter" prompt="Minimal 8 karakter" sqref="D1:D1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Awali dengan kode negara 62" sqref="E1:E1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Referensi" prompt="Admin : 1_x000a_Guru : 2_x000a_Siswa : 3" sqref="F1:F1048576"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" error="Minimal 8 karakter" prompt="Minimal 8 karakter" sqref="E1:E1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Awali dengan kode negara 62" sqref="F1:F1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Referensi" prompt="Admin : 1_x000a_Guru : 2_x000a_Siswa : 3" sqref="G1:G1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>